<commit_message>
Adding of GUI-Message-Box support -Franz Zeilinger
</commit_message>
<xml_diff>
--- a/1_Program/Datastructure - GAT.xlsx
+++ b/1_Program/Datastructure - GAT.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>handles</t>
   </si>
@@ -135,6 +135,21 @@
   </si>
   <si>
     <t>% Typen der Wochentage; 1.Spalte programminterne Bezeichnung, 2.Spalte Bezeichnung für User / Ausgabe</t>
+  </si>
+  <si>
+    <t>.Main_Path</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>% Pfad, in dem sich NAT_main.m befindet und daher das Programm ausgeführt wird.</t>
+  </si>
+  <si>
+    <t>.Files</t>
+  </si>
+  <si>
+    <t>% Einstellungen sämtliche Dateien, auf die zugegriffen wird, betreffend</t>
   </si>
 </sst>
 </file>
@@ -806,10 +821,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:CE279"/>
+  <dimension ref="A1:CE281"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W14" sqref="W14"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,12 +847,12 @@
     <col min="59" max="16384" width="3.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
@@ -845,7 +860,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
@@ -856,92 +871,130 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+    <row r="4" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="D4" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="U4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="BJ4" s="12"/>
+      <c r="BK4" s="12"/>
+      <c r="BU4" s="13"/>
+      <c r="BY4" s="5"/>
+      <c r="BZ4" s="5"/>
+      <c r="CA4" s="5"/>
+      <c r="CB4" s="5"/>
+      <c r="CC4" s="5"/>
+      <c r="CD4" s="5"/>
+      <c r="CE4" s="5"/>
+    </row>
+    <row r="5" spans="1:83" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="C5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="E5" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="V5" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="O7" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U5" s="5" t="s">
+      <c r="U7" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="8" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="17" t="s">
+      <c r="C8" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="O6" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="U6" s="5" t="s">
+      <c r="U8" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D8" s="20"/>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D9" s="20"/>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D10" s="20"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D11" s="20"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D12" s="20"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D13" s="20"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D14" s="20"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D15" s="20"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:83" x14ac:dyDescent="0.25">
       <c r="D16" s="20"/>
     </row>
     <row r="17" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D17" s="19"/>
+      <c r="D17" s="20"/>
     </row>
     <row r="18" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D18" s="20"/>
     </row>
     <row r="19" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D19" s="20"/>
+      <c r="D19" s="19"/>
     </row>
     <row r="20" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D20" s="19"/>
+      <c r="D20" s="20"/>
     </row>
     <row r="21" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D21" s="20"/>
@@ -954,10 +1007,9 @@
     </row>
     <row r="24" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D24" s="19"/>
-      <c r="E24" s="23"/>
     </row>
     <row r="25" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D25" s="19"/>
+      <c r="D25" s="20"/>
     </row>
     <row r="26" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D26" s="19"/>
@@ -969,59 +1021,48 @@
     <row r="28" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D28" s="19"/>
       <c r="E28" s="23"/>
-      <c r="W28" s="54"/>
     </row>
     <row r="29" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D29" s="19"/>
-      <c r="E29" s="22"/>
-      <c r="F29" s="41"/>
-      <c r="X29" s="54"/>
     </row>
     <row r="30" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D30" s="19"/>
-      <c r="E30" s="22"/>
-      <c r="F30" s="41"/>
-      <c r="V30" s="3"/>
+      <c r="E30" s="23"/>
+      <c r="W30" s="54"/>
     </row>
     <row r="31" spans="4:24" x14ac:dyDescent="0.25">
-      <c r="D31" s="20"/>
+      <c r="D31" s="19"/>
       <c r="E31" s="22"/>
       <c r="F31" s="41"/>
+      <c r="X31" s="54"/>
     </row>
     <row r="32" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D32" s="19"/>
       <c r="E32" s="22"/>
       <c r="F32" s="41"/>
-    </row>
-    <row r="33" spans="4:51" x14ac:dyDescent="0.25">
+      <c r="V32" s="3"/>
+    </row>
+    <row r="33" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D33" s="20"/>
-      <c r="W33" s="3"/>
-    </row>
-    <row r="34" spans="4:51" x14ac:dyDescent="0.25">
-      <c r="D34" s="20"/>
-      <c r="W34" s="3"/>
-    </row>
-    <row r="35" spans="4:51" x14ac:dyDescent="0.25">
-      <c r="D35" s="19"/>
-      <c r="E35" s="23"/>
-      <c r="Z35" s="5"/>
-      <c r="AA35" s="5"/>
-      <c r="AB35" s="5"/>
-      <c r="AC35" s="5"/>
-      <c r="AD35" s="5"/>
-      <c r="AE35" s="5"/>
-    </row>
-    <row r="36" spans="4:51" x14ac:dyDescent="0.25">
-      <c r="D36" s="19"/>
-      <c r="Z36" s="5"/>
-      <c r="AA36" s="5"/>
-      <c r="AB36" s="5"/>
-      <c r="AC36" s="5"/>
-      <c r="AD36" s="5"/>
-      <c r="AE36" s="5"/>
-    </row>
-    <row r="37" spans="4:51" x14ac:dyDescent="0.25">
+      <c r="E33" s="22"/>
+      <c r="F33" s="41"/>
+    </row>
+    <row r="34" spans="4:38" x14ac:dyDescent="0.25">
+      <c r="D34" s="19"/>
+      <c r="E34" s="22"/>
+      <c r="F34" s="41"/>
+    </row>
+    <row r="35" spans="4:38" x14ac:dyDescent="0.25">
+      <c r="D35" s="20"/>
+      <c r="W35" s="3"/>
+    </row>
+    <row r="36" spans="4:38" x14ac:dyDescent="0.25">
+      <c r="D36" s="20"/>
+      <c r="W36" s="3"/>
+    </row>
+    <row r="37" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D37" s="19"/>
+      <c r="E37" s="23"/>
       <c r="Z37" s="5"/>
       <c r="AA37" s="5"/>
       <c r="AB37" s="5"/>
@@ -1029,7 +1070,7 @@
       <c r="AD37" s="5"/>
       <c r="AE37" s="5"/>
     </row>
-    <row r="38" spans="4:51" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D38" s="19"/>
       <c r="Z38" s="5"/>
       <c r="AA38" s="5"/>
@@ -1038,139 +1079,149 @@
       <c r="AD38" s="5"/>
       <c r="AE38" s="5"/>
     </row>
-    <row r="39" spans="4:51" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D39" s="19"/>
-      <c r="W39" s="3"/>
-      <c r="Y39" s="47"/>
-    </row>
-    <row r="40" spans="4:51" x14ac:dyDescent="0.25">
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="5"/>
+      <c r="AC39" s="5"/>
+      <c r="AD39" s="5"/>
+      <c r="AE39" s="5"/>
+    </row>
+    <row r="40" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D40" s="19"/>
-      <c r="W40" s="3"/>
-    </row>
-    <row r="41" spans="4:51" x14ac:dyDescent="0.25">
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="5"/>
+      <c r="AC40" s="5"/>
+      <c r="AD40" s="5"/>
+      <c r="AE40" s="5"/>
+    </row>
+    <row r="41" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D41" s="19"/>
       <c r="W41" s="3"/>
-      <c r="Z41" s="5"/>
-    </row>
-    <row r="42" spans="4:51" x14ac:dyDescent="0.25">
-      <c r="D42" s="20"/>
+      <c r="Y41" s="47"/>
+    </row>
+    <row r="42" spans="4:38" x14ac:dyDescent="0.25">
+      <c r="D42" s="19"/>
       <c r="W42" s="3"/>
-      <c r="Z42" s="5"/>
-    </row>
-    <row r="43" spans="4:51" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D43" s="19"/>
       <c r="W43" s="3"/>
       <c r="Z43" s="5"/>
     </row>
-    <row r="44" spans="4:51" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D44" s="20"/>
       <c r="W44" s="3"/>
       <c r="Z44" s="5"/>
     </row>
-    <row r="45" spans="4:51" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:38" x14ac:dyDescent="0.25">
       <c r="D45" s="19"/>
-      <c r="E45" s="23"/>
+      <c r="W45" s="3"/>
       <c r="Z45" s="5"/>
-      <c r="AA45" s="5"/>
-      <c r="AB45" s="5"/>
-      <c r="AC45" s="5"/>
-      <c r="AD45" s="5"/>
-      <c r="AE45" s="5"/>
-      <c r="AF45" s="5"/>
-      <c r="AG45" s="5"/>
-      <c r="AH45" s="5"/>
-      <c r="AI45" s="5"/>
-      <c r="AJ45" s="5"/>
-      <c r="AK45" s="5"/>
-      <c r="AL45" s="5"/>
-    </row>
-    <row r="46" spans="4:51" x14ac:dyDescent="0.25">
-      <c r="D46" s="19"/>
+    </row>
+    <row r="46" spans="4:38" x14ac:dyDescent="0.25">
+      <c r="D46" s="20"/>
+      <c r="W46" s="3"/>
       <c r="Z46" s="5"/>
-      <c r="AA46" s="5"/>
-      <c r="AB46" s="5"/>
-      <c r="AC46" s="5"/>
-      <c r="AD46" s="5"/>
-      <c r="AE46" s="5"/>
-      <c r="AF46" s="5"/>
-      <c r="AG46" s="5"/>
-      <c r="AH46" s="5"/>
-      <c r="AI46" s="5"/>
-      <c r="AJ46" s="5"/>
-      <c r="AK46" s="5"/>
-      <c r="AL46" s="5"/>
-    </row>
-    <row r="47" spans="4:51" x14ac:dyDescent="0.25">
-      <c r="D47" s="20"/>
-      <c r="F47" s="42"/>
-      <c r="X47" s="11"/>
-      <c r="Y47" s="11"/>
-      <c r="Z47" s="11"/>
-      <c r="AA47" s="11"/>
-      <c r="AB47" s="11"/>
-      <c r="AC47" s="11"/>
-      <c r="AD47" s="11"/>
-      <c r="AE47" s="11"/>
-      <c r="AF47" s="11"/>
-      <c r="AG47" s="11"/>
-      <c r="AH47" s="11"/>
-      <c r="AI47" s="11"/>
-      <c r="AJ47" s="11"/>
-      <c r="AK47" s="11"/>
-      <c r="AL47" s="11"/>
-      <c r="AM47" s="11"/>
-      <c r="AN47" s="11"/>
-      <c r="AO47" s="11"/>
-      <c r="AP47" s="11"/>
-      <c r="AQ47" s="11"/>
-      <c r="AR47" s="11"/>
-      <c r="AS47" s="11"/>
-      <c r="AT47" s="11"/>
-      <c r="AU47" s="11"/>
-      <c r="AV47" s="11"/>
-      <c r="AW47" s="11"/>
-      <c r="AX47" s="11"/>
-      <c r="AY47" s="5"/>
-    </row>
-    <row r="48" spans="4:51" x14ac:dyDescent="0.25">
-      <c r="D48" s="20"/>
-      <c r="F48" s="42"/>
-      <c r="X48" s="11"/>
-      <c r="Y48" s="11"/>
-      <c r="Z48" s="11"/>
-      <c r="AA48" s="11"/>
-      <c r="AB48" s="11"/>
-      <c r="AC48" s="11"/>
-      <c r="AD48" s="11"/>
-      <c r="AE48" s="11"/>
-      <c r="AF48" s="11"/>
-      <c r="AG48" s="11"/>
-      <c r="AH48" s="11"/>
-      <c r="AI48" s="11"/>
-      <c r="AJ48" s="11"/>
-      <c r="AK48" s="11"/>
-      <c r="AL48" s="11"/>
-      <c r="AM48" s="11"/>
-      <c r="AN48" s="11"/>
-      <c r="AO48" s="11"/>
-      <c r="AP48" s="11"/>
-      <c r="AQ48" s="11"/>
-      <c r="AR48" s="11"/>
-      <c r="AS48" s="11"/>
-      <c r="AT48" s="11"/>
-      <c r="AU48" s="11"/>
-      <c r="AV48" s="11"/>
-      <c r="AW48" s="11"/>
-      <c r="AX48" s="11"/>
-      <c r="AY48" s="5"/>
+    </row>
+    <row r="47" spans="4:38" x14ac:dyDescent="0.25">
+      <c r="D47" s="19"/>
+      <c r="E47" s="23"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="5"/>
+      <c r="AE47" s="5"/>
+      <c r="AF47" s="5"/>
+      <c r="AG47" s="5"/>
+      <c r="AH47" s="5"/>
+      <c r="AI47" s="5"/>
+      <c r="AJ47" s="5"/>
+      <c r="AK47" s="5"/>
+      <c r="AL47" s="5"/>
+    </row>
+    <row r="48" spans="4:38" x14ac:dyDescent="0.25">
+      <c r="D48" s="19"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5"/>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="5"/>
+      <c r="AE48" s="5"/>
+      <c r="AF48" s="5"/>
+      <c r="AG48" s="5"/>
+      <c r="AH48" s="5"/>
+      <c r="AI48" s="5"/>
+      <c r="AJ48" s="5"/>
+      <c r="AK48" s="5"/>
+      <c r="AL48" s="5"/>
     </row>
     <row r="49" spans="3:83" x14ac:dyDescent="0.25">
-      <c r="D49" s="19"/>
-      <c r="W49" s="3"/>
+      <c r="D49" s="20"/>
+      <c r="F49" s="42"/>
+      <c r="X49" s="11"/>
+      <c r="Y49" s="11"/>
+      <c r="Z49" s="11"/>
+      <c r="AA49" s="11"/>
+      <c r="AB49" s="11"/>
+      <c r="AC49" s="11"/>
+      <c r="AD49" s="11"/>
+      <c r="AE49" s="11"/>
+      <c r="AF49" s="11"/>
+      <c r="AG49" s="11"/>
+      <c r="AH49" s="11"/>
+      <c r="AI49" s="11"/>
+      <c r="AJ49" s="11"/>
+      <c r="AK49" s="11"/>
+      <c r="AL49" s="11"/>
+      <c r="AM49" s="11"/>
+      <c r="AN49" s="11"/>
+      <c r="AO49" s="11"/>
+      <c r="AP49" s="11"/>
+      <c r="AQ49" s="11"/>
+      <c r="AR49" s="11"/>
+      <c r="AS49" s="11"/>
+      <c r="AT49" s="11"/>
+      <c r="AU49" s="11"/>
+      <c r="AV49" s="11"/>
+      <c r="AW49" s="11"/>
+      <c r="AX49" s="11"/>
+      <c r="AY49" s="5"/>
     </row>
     <row r="50" spans="3:83" x14ac:dyDescent="0.25">
-      <c r="D50" s="19"/>
-      <c r="W50" s="3"/>
+      <c r="D50" s="20"/>
+      <c r="F50" s="42"/>
+      <c r="X50" s="11"/>
+      <c r="Y50" s="11"/>
+      <c r="Z50" s="11"/>
+      <c r="AA50" s="11"/>
+      <c r="AB50" s="11"/>
+      <c r="AC50" s="11"/>
+      <c r="AD50" s="11"/>
+      <c r="AE50" s="11"/>
+      <c r="AF50" s="11"/>
+      <c r="AG50" s="11"/>
+      <c r="AH50" s="11"/>
+      <c r="AI50" s="11"/>
+      <c r="AJ50" s="11"/>
+      <c r="AK50" s="11"/>
+      <c r="AL50" s="11"/>
+      <c r="AM50" s="11"/>
+      <c r="AN50" s="11"/>
+      <c r="AO50" s="11"/>
+      <c r="AP50" s="11"/>
+      <c r="AQ50" s="11"/>
+      <c r="AR50" s="11"/>
+      <c r="AS50" s="11"/>
+      <c r="AT50" s="11"/>
+      <c r="AU50" s="11"/>
+      <c r="AV50" s="11"/>
+      <c r="AW50" s="11"/>
+      <c r="AX50" s="11"/>
+      <c r="AY50" s="5"/>
     </row>
     <row r="51" spans="3:83" x14ac:dyDescent="0.25">
       <c r="D51" s="19"/>
@@ -1189,80 +1240,82 @@
       <c r="W54" s="3"/>
     </row>
     <row r="55" spans="3:83" x14ac:dyDescent="0.25">
-      <c r="D55" s="20"/>
+      <c r="D55" s="19"/>
       <c r="W55" s="3"/>
     </row>
     <row r="56" spans="3:83" x14ac:dyDescent="0.25">
       <c r="D56" s="19"/>
-      <c r="BJ56" s="12"/>
-      <c r="BK56" s="12"/>
-      <c r="BU56" s="13"/>
-      <c r="BY56" s="5"/>
-      <c r="BZ56" s="5"/>
-      <c r="CA56" s="5"/>
-      <c r="CB56" s="5"/>
-      <c r="CC56" s="5"/>
-      <c r="CD56" s="5"/>
-      <c r="CE56" s="5"/>
+      <c r="W56" s="3"/>
     </row>
     <row r="57" spans="3:83" x14ac:dyDescent="0.25">
-      <c r="C57" s="17"/>
-      <c r="D57" s="19"/>
-      <c r="BJ57" s="12"/>
-      <c r="BK57" s="12"/>
-      <c r="BU57" s="13"/>
-      <c r="BY57" s="5"/>
-      <c r="BZ57" s="5"/>
-      <c r="CA57" s="5"/>
-      <c r="CB57" s="5"/>
-      <c r="CC57" s="5"/>
-      <c r="CD57" s="5"/>
-      <c r="CE57" s="5"/>
+      <c r="D57" s="20"/>
+      <c r="W57" s="3"/>
+    </row>
+    <row r="58" spans="3:83" x14ac:dyDescent="0.25">
+      <c r="D58" s="19"/>
+      <c r="BJ58" s="12"/>
+      <c r="BK58" s="12"/>
+      <c r="BU58" s="13"/>
+      <c r="BY58" s="5"/>
+      <c r="BZ58" s="5"/>
+      <c r="CA58" s="5"/>
+      <c r="CB58" s="5"/>
+      <c r="CC58" s="5"/>
+      <c r="CD58" s="5"/>
+      <c r="CE58" s="5"/>
     </row>
     <row r="59" spans="3:83" x14ac:dyDescent="0.25">
-      <c r="D59" s="20"/>
-    </row>
-    <row r="60" spans="3:83" x14ac:dyDescent="0.25">
-      <c r="D60" s="19"/>
+      <c r="C59" s="17"/>
+      <c r="D59" s="19"/>
+      <c r="BJ59" s="12"/>
+      <c r="BK59" s="12"/>
+      <c r="BU59" s="13"/>
+      <c r="BY59" s="5"/>
+      <c r="BZ59" s="5"/>
+      <c r="CA59" s="5"/>
+      <c r="CB59" s="5"/>
+      <c r="CC59" s="5"/>
+      <c r="CD59" s="5"/>
+      <c r="CE59" s="5"/>
     </row>
     <row r="61" spans="3:83" x14ac:dyDescent="0.25">
       <c r="D61" s="20"/>
-      <c r="E61" s="22"/>
-      <c r="F61" s="41"/>
     </row>
     <row r="62" spans="3:83" x14ac:dyDescent="0.25">
       <c r="D62" s="19"/>
     </row>
     <row r="63" spans="3:83" x14ac:dyDescent="0.25">
-      <c r="D63" s="19"/>
+      <c r="D63" s="20"/>
+      <c r="E63" s="22"/>
+      <c r="F63" s="41"/>
     </row>
     <row r="64" spans="3:83" x14ac:dyDescent="0.25">
       <c r="D64" s="19"/>
     </row>
     <row r="65" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D65" s="19"/>
-      <c r="E65" s="22"/>
-      <c r="F65" s="41"/>
     </row>
     <row r="66" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D66" s="19"/>
     </row>
     <row r="67" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D67" s="19"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="41"/>
     </row>
     <row r="68" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D68" s="19"/>
     </row>
     <row r="69" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D69" s="19"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="41"/>
     </row>
     <row r="70" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D70" s="19"/>
     </row>
     <row r="71" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D71" s="19"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="41"/>
     </row>
     <row r="72" spans="4:6" x14ac:dyDescent="0.25">
       <c r="D72" s="19"/>
@@ -1292,7 +1345,6 @@
       <c r="D80" s="19"/>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C81" s="17"/>
       <c r="D81" s="19"/>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
@@ -1300,33 +1352,34 @@
     </row>
     <row r="83" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C83" s="17"/>
+      <c r="D83" s="19"/>
     </row>
     <row r="84" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D84" s="20"/>
+      <c r="D84" s="19"/>
     </row>
     <row r="85" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D85" s="20"/>
+      <c r="C85" s="17"/>
     </row>
     <row r="86" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D86" s="20"/>
     </row>
     <row r="87" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D87" s="19"/>
+      <c r="D87" s="20"/>
     </row>
     <row r="88" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D88" s="19"/>
+      <c r="D88" s="20"/>
     </row>
     <row r="89" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D89" s="19"/>
     </row>
     <row r="90" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D90" s="20"/>
+      <c r="D90" s="19"/>
     </row>
     <row r="91" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D91" s="19"/>
     </row>
     <row r="92" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D92" s="19"/>
+      <c r="D92" s="20"/>
     </row>
     <row r="93" spans="3:4" x14ac:dyDescent="0.25">
       <c r="D93" s="19"/>
@@ -1335,62 +1388,60 @@
       <c r="D94" s="19"/>
     </row>
     <row r="95" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C95" s="17"/>
+      <c r="D95" s="19"/>
     </row>
     <row r="96" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D96" s="20"/>
-    </row>
-    <row r="97" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D97" s="19"/>
-    </row>
-    <row r="98" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D98" s="19"/>
-    </row>
-    <row r="99" spans="4:21" x14ac:dyDescent="0.25">
+      <c r="D96" s="19"/>
+    </row>
+    <row r="97" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C97" s="17"/>
+    </row>
+    <row r="98" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D98" s="20"/>
+    </row>
+    <row r="99" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D99" s="19"/>
     </row>
-    <row r="100" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="100" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D100" s="19"/>
     </row>
-    <row r="101" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="101" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D101" s="19"/>
     </row>
-    <row r="102" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="102" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D102" s="19"/>
     </row>
-    <row r="103" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D103" s="20"/>
-    </row>
-    <row r="104" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="103" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D103" s="19"/>
+    </row>
+    <row r="104" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D104" s="19"/>
     </row>
-    <row r="105" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="105" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D105" s="20"/>
     </row>
-    <row r="106" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="106" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D106" s="19"/>
     </row>
-    <row r="107" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="107" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D107" s="20"/>
-      <c r="U107" s="3"/>
-    </row>
-    <row r="108" spans="4:21" x14ac:dyDescent="0.25">
+    </row>
+    <row r="108" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D108" s="19"/>
-      <c r="U108" s="3"/>
-    </row>
-    <row r="109" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D109" s="19"/>
+    </row>
+    <row r="109" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D109" s="20"/>
       <c r="U109" s="3"/>
     </row>
-    <row r="110" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D110" s="20"/>
+    <row r="110" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D110" s="19"/>
       <c r="U110" s="3"/>
     </row>
-    <row r="111" spans="4:21" x14ac:dyDescent="0.25">
-      <c r="D111" s="20"/>
+    <row r="111" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="D111" s="19"/>
       <c r="U111" s="3"/>
     </row>
-    <row r="112" spans="4:21" x14ac:dyDescent="0.25">
+    <row r="112" spans="3:21" x14ac:dyDescent="0.25">
       <c r="D112" s="20"/>
       <c r="U112" s="3"/>
     </row>
@@ -1424,19 +1475,21 @@
     </row>
     <row r="120" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D120" s="20"/>
+      <c r="U120" s="3"/>
     </row>
     <row r="121" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D121" s="20"/>
+      <c r="U121" s="3"/>
     </row>
     <row r="122" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D122" s="19"/>
-      <c r="V122" s="3"/>
+      <c r="D122" s="20"/>
     </row>
     <row r="123" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D123" s="20"/>
     </row>
     <row r="124" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D124" s="20"/>
+      <c r="D124" s="19"/>
+      <c r="V124" s="3"/>
     </row>
     <row r="125" spans="4:22" x14ac:dyDescent="0.25">
       <c r="D125" s="20"/>
@@ -1448,17 +1501,17 @@
       <c r="D127" s="20"/>
     </row>
     <row r="128" spans="4:22" x14ac:dyDescent="0.25">
-      <c r="D128" s="19"/>
+      <c r="D128" s="20"/>
     </row>
     <row r="129" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C129" s="8"/>
-      <c r="D129" s="19"/>
+      <c r="D129" s="20"/>
     </row>
     <row r="130" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D130" s="20"/>
+      <c r="D130" s="19"/>
     </row>
     <row r="131" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D131" s="20"/>
+      <c r="C131" s="8"/>
+      <c r="D131" s="19"/>
     </row>
     <row r="132" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D132" s="20"/>
@@ -1476,28 +1529,28 @@
       <c r="D136" s="20"/>
     </row>
     <row r="137" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D137" s="19"/>
+      <c r="D137" s="20"/>
     </row>
     <row r="138" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B138" s="9"/>
-      <c r="D138" s="19"/>
+      <c r="D138" s="20"/>
     </row>
     <row r="139" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D139" s="19"/>
     </row>
     <row r="140" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C140" s="17"/>
+      <c r="B140" s="9"/>
       <c r="D140" s="19"/>
     </row>
     <row r="141" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="C141" s="17"/>
       <c r="D141" s="19"/>
     </row>
     <row r="142" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D142" s="20"/>
+      <c r="C142" s="17"/>
+      <c r="D142" s="19"/>
     </row>
     <row r="143" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="D143" s="20"/>
+      <c r="C143" s="17"/>
+      <c r="D143" s="19"/>
     </row>
     <row r="144" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D144" s="20"/>
@@ -1507,13 +1560,13 @@
     </row>
     <row r="146" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D146" s="20"/>
-      <c r="G146" s="3"/>
     </row>
     <row r="147" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D147" s="20"/>
     </row>
     <row r="148" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D148" s="20"/>
+      <c r="G148" s="3"/>
     </row>
     <row r="149" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D149" s="20"/>
@@ -1535,20 +1588,20 @@
     </row>
     <row r="155" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D155" s="20"/>
-      <c r="V155" s="3"/>
     </row>
     <row r="156" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D156" s="20"/>
     </row>
     <row r="157" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="C157" s="17"/>
-      <c r="D157" s="19"/>
+      <c r="D157" s="20"/>
+      <c r="V157" s="3"/>
     </row>
     <row r="158" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D158" s="20"/>
     </row>
     <row r="159" spans="3:22" x14ac:dyDescent="0.25">
-      <c r="D159" s="20"/>
+      <c r="C159" s="17"/>
+      <c r="D159" s="19"/>
     </row>
     <row r="160" spans="3:22" x14ac:dyDescent="0.25">
       <c r="D160" s="20"/>
@@ -1578,13 +1631,13 @@
       <c r="D168" s="20"/>
     </row>
     <row r="169" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D169" s="3"/>
+      <c r="D169" s="20"/>
     </row>
     <row r="170" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D170" s="20"/>
     </row>
     <row r="171" spans="4:4" x14ac:dyDescent="0.25">
-      <c r="D171" s="20"/>
+      <c r="D171" s="3"/>
     </row>
     <row r="172" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D172" s="20"/>
@@ -1608,25 +1661,25 @@
       <c r="D178" s="20"/>
     </row>
     <row r="179" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D179" s="19"/>
+      <c r="D179" s="20"/>
     </row>
     <row r="180" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D180" s="19"/>
-      <c r="F180" s="41"/>
-      <c r="X180" s="3"/>
-      <c r="AA180" s="5"/>
+      <c r="D180" s="20"/>
     </row>
     <row r="181" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D181" s="19"/>
-      <c r="F181" s="41"/>
-      <c r="X181" s="3"/>
-      <c r="AA181" s="5"/>
     </row>
     <row r="182" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D182" s="20"/>
+      <c r="D182" s="19"/>
+      <c r="F182" s="41"/>
+      <c r="X182" s="3"/>
+      <c r="AA182" s="5"/>
     </row>
     <row r="183" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D183" s="20"/>
+      <c r="D183" s="19"/>
+      <c r="F183" s="41"/>
+      <c r="X183" s="3"/>
+      <c r="AA183" s="5"/>
     </row>
     <row r="184" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D184" s="20"/>
@@ -1644,75 +1697,69 @@
       <c r="D188" s="20"/>
     </row>
     <row r="189" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D189" s="19"/>
-      <c r="X189" s="3"/>
-      <c r="AA189" s="5"/>
+      <c r="D189" s="20"/>
     </row>
     <row r="190" spans="4:27" x14ac:dyDescent="0.25">
-      <c r="D190" s="19"/>
-      <c r="F190" s="41"/>
-      <c r="X190" s="3"/>
-      <c r="AA190" s="5"/>
+      <c r="D190" s="20"/>
     </row>
     <row r="191" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D191" s="19"/>
+      <c r="X191" s="3"/>
+      <c r="AA191" s="5"/>
     </row>
     <row r="192" spans="4:27" x14ac:dyDescent="0.25">
       <c r="D192" s="19"/>
+      <c r="F192" s="41"/>
+      <c r="X192" s="3"/>
+      <c r="AA192" s="5"/>
     </row>
     <row r="193" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="C193" s="17"/>
       <c r="D193" s="19"/>
     </row>
     <row r="194" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="D194" s="20"/>
+      <c r="D194" s="19"/>
     </row>
     <row r="195" spans="2:39" x14ac:dyDescent="0.25">
+      <c r="C195" s="17"/>
       <c r="D195" s="19"/>
     </row>
     <row r="196" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="C196" s="8"/>
-      <c r="D196" s="19"/>
+      <c r="D196" s="20"/>
     </row>
     <row r="197" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="C197" s="8"/>
-      <c r="D197" s="20"/>
+      <c r="D197" s="19"/>
     </row>
     <row r="198" spans="2:39" x14ac:dyDescent="0.25">
       <c r="C198" s="8"/>
       <c r="D198" s="19"/>
     </row>
     <row r="199" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="B199" s="9"/>
-      <c r="D199" s="19"/>
-      <c r="E199" s="3"/>
-      <c r="F199" s="3"/>
-      <c r="AM199" s="14"/>
+      <c r="C199" s="8"/>
+      <c r="D199" s="20"/>
     </row>
     <row r="200" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="B200" s="9"/>
       <c r="C200" s="8"/>
+      <c r="D200" s="19"/>
     </row>
     <row r="201" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="C201" s="17"/>
+      <c r="B201" s="9"/>
+      <c r="D201" s="19"/>
+      <c r="E201" s="3"/>
+      <c r="F201" s="3"/>
+      <c r="AM201" s="14"/>
     </row>
     <row r="202" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="D202" s="20"/>
+      <c r="B202" s="9"/>
+      <c r="C202" s="8"/>
     </row>
     <row r="203" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="D203" s="20"/>
+      <c r="C203" s="17"/>
     </row>
     <row r="204" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D204" s="20"/>
-      <c r="U204" s="3"/>
-      <c r="X204" s="3"/>
-      <c r="Y204" s="3"/>
     </row>
     <row r="205" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D205" s="20"/>
-      <c r="U205" s="3"/>
-      <c r="X205" s="3"/>
-      <c r="Y205" s="3"/>
     </row>
     <row r="206" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D206" s="20"/>
@@ -1723,7 +1770,8 @@
     <row r="207" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D207" s="20"/>
       <c r="U207" s="3"/>
-      <c r="Z207" s="5"/>
+      <c r="X207" s="3"/>
+      <c r="Y207" s="3"/>
     </row>
     <row r="208" spans="2:39" x14ac:dyDescent="0.25">
       <c r="D208" s="20"/>
@@ -1731,155 +1779,128 @@
       <c r="X208" s="3"/>
       <c r="Y208" s="3"/>
     </row>
-    <row r="209" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="209" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D209" s="20"/>
       <c r="U209" s="3"/>
-      <c r="X209" s="3"/>
-      <c r="Y209" s="3"/>
-    </row>
-    <row r="210" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D210" s="19"/>
+      <c r="Z209" s="5"/>
+    </row>
+    <row r="210" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D210" s="20"/>
       <c r="U210" s="3"/>
       <c r="X210" s="3"/>
       <c r="Y210" s="3"/>
     </row>
-    <row r="211" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="211" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D211" s="20"/>
       <c r="U211" s="3"/>
       <c r="X211" s="3"/>
       <c r="Y211" s="3"/>
     </row>
-    <row r="212" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="D212" s="20"/>
+    <row r="212" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D212" s="19"/>
       <c r="U212" s="3"/>
       <c r="X212" s="3"/>
       <c r="Y212" s="3"/>
     </row>
-    <row r="213" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="213" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D213" s="20"/>
       <c r="U213" s="3"/>
       <c r="X213" s="3"/>
       <c r="Y213" s="3"/>
     </row>
-    <row r="214" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="214" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D214" s="20"/>
       <c r="U214" s="3"/>
       <c r="X214" s="3"/>
       <c r="Y214" s="3"/>
     </row>
-    <row r="215" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="215" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D215" s="20"/>
       <c r="U215" s="3"/>
       <c r="X215" s="3"/>
       <c r="Y215" s="3"/>
     </row>
-    <row r="216" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="216" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D216" s="20"/>
       <c r="U216" s="3"/>
       <c r="X216" s="3"/>
       <c r="Y216" s="3"/>
     </row>
-    <row r="217" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="217" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D217" s="20"/>
       <c r="U217" s="3"/>
       <c r="X217" s="3"/>
       <c r="Y217" s="3"/>
     </row>
-    <row r="218" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="218" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D218" s="20"/>
       <c r="U218" s="3"/>
       <c r="X218" s="3"/>
       <c r="Y218" s="3"/>
     </row>
-    <row r="219" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="219" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D219" s="20"/>
       <c r="U219" s="3"/>
       <c r="X219" s="3"/>
       <c r="Y219" s="3"/>
     </row>
-    <row r="220" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="220" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D220" s="20"/>
       <c r="U220" s="3"/>
       <c r="X220" s="3"/>
       <c r="Y220" s="3"/>
     </row>
-    <row r="221" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="221" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D221" s="20"/>
       <c r="U221" s="3"/>
       <c r="X221" s="3"/>
       <c r="Y221" s="3"/>
     </row>
-    <row r="222" spans="3:29" x14ac:dyDescent="0.25">
+    <row r="222" spans="4:26" x14ac:dyDescent="0.25">
       <c r="D222" s="20"/>
       <c r="U222" s="3"/>
       <c r="X222" s="3"/>
       <c r="Y222" s="3"/>
     </row>
-    <row r="223" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="C223" s="17"/>
-      <c r="Z223" s="5"/>
-      <c r="AA223" s="5"/>
-      <c r="AB223" s="5"/>
-      <c r="AC223" s="5"/>
-    </row>
-    <row r="224" spans="3:29" x14ac:dyDescent="0.25">
-      <c r="Z224" s="5"/>
-      <c r="AA224" s="5"/>
-      <c r="AB224" s="5"/>
-      <c r="AC224" s="5"/>
+    <row r="223" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D223" s="20"/>
+      <c r="U223" s="3"/>
+      <c r="X223" s="3"/>
+      <c r="Y223" s="3"/>
+    </row>
+    <row r="224" spans="4:26" x14ac:dyDescent="0.25">
+      <c r="D224" s="20"/>
+      <c r="U224" s="3"/>
+      <c r="X224" s="3"/>
+      <c r="Y224" s="3"/>
     </row>
     <row r="225" spans="2:58" x14ac:dyDescent="0.25">
       <c r="C225" s="17"/>
+      <c r="Z225" s="5"/>
+      <c r="AA225" s="5"/>
+      <c r="AB225" s="5"/>
+      <c r="AC225" s="5"/>
     </row>
     <row r="226" spans="2:58" x14ac:dyDescent="0.25">
-      <c r="C226" s="17"/>
+      <c r="Z226" s="5"/>
+      <c r="AA226" s="5"/>
+      <c r="AB226" s="5"/>
+      <c r="AC226" s="5"/>
     </row>
     <row r="227" spans="2:58" x14ac:dyDescent="0.25">
       <c r="C227" s="17"/>
     </row>
-    <row r="228" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B228" s="2"/>
-      <c r="C228" s="24"/>
-      <c r="D228" s="33"/>
-      <c r="E228" s="36"/>
-      <c r="F228" s="43"/>
-      <c r="G228" s="43"/>
-      <c r="H228" s="49"/>
-      <c r="I228" s="52"/>
-      <c r="O228" s="27"/>
-      <c r="S228" s="28"/>
-      <c r="T228" s="28"/>
-      <c r="U228" s="28"/>
-      <c r="V228" s="28"/>
-      <c r="W228" s="28"/>
-      <c r="X228" s="28"/>
-      <c r="Y228" s="28"/>
-      <c r="BF228" s="29"/>
-    </row>
-    <row r="229" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B229" s="2"/>
-      <c r="C229" s="30"/>
-      <c r="D229" s="31"/>
-      <c r="E229" s="36"/>
-      <c r="F229" s="43"/>
-      <c r="G229" s="43"/>
-      <c r="H229" s="49"/>
-      <c r="I229" s="52"/>
-      <c r="O229" s="27"/>
-      <c r="S229" s="28"/>
-      <c r="T229" s="28"/>
-      <c r="U229" s="28"/>
-      <c r="V229" s="28"/>
-      <c r="W229" s="28"/>
-      <c r="X229" s="28"/>
-      <c r="Y229" s="28"/>
-      <c r="BF229" s="29"/>
+    <row r="228" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="C228" s="17"/>
+    </row>
+    <row r="229" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="C229" s="17"/>
     </row>
     <row r="230" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B230" s="2"/>
-      <c r="C230" s="30"/>
-      <c r="D230" s="25"/>
-      <c r="E230" s="37"/>
+      <c r="C230" s="24"/>
+      <c r="D230" s="33"/>
+      <c r="E230" s="36"/>
       <c r="F230" s="43"/>
       <c r="G230" s="43"/>
       <c r="H230" s="49"/>
@@ -1892,14 +1913,13 @@
       <c r="W230" s="28"/>
       <c r="X230" s="28"/>
       <c r="Y230" s="28"/>
-      <c r="AQ230" s="28"/>
       <c r="BF230" s="29"/>
     </row>
     <row r="231" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B231" s="2"/>
       <c r="C231" s="30"/>
-      <c r="D231" s="25"/>
-      <c r="E231" s="37"/>
+      <c r="D231" s="31"/>
+      <c r="E231" s="36"/>
       <c r="F231" s="43"/>
       <c r="G231" s="43"/>
       <c r="H231" s="49"/>
@@ -1912,7 +1932,6 @@
       <c r="W231" s="28"/>
       <c r="X231" s="28"/>
       <c r="Y231" s="28"/>
-      <c r="AQ231" s="28"/>
       <c r="BF231" s="29"/>
     </row>
     <row r="232" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -1973,7 +1992,6 @@
       <c r="X234" s="28"/>
       <c r="Y234" s="28"/>
       <c r="AQ234" s="28"/>
-      <c r="AR234" s="28"/>
       <c r="BF234" s="29"/>
     </row>
     <row r="235" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -1994,8 +2012,6 @@
       <c r="X235" s="28"/>
       <c r="Y235" s="28"/>
       <c r="AQ235" s="28"/>
-      <c r="AR235" s="28"/>
-      <c r="AY235" s="35"/>
       <c r="BF235" s="29"/>
     </row>
     <row r="236" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2016,7 +2032,7 @@
       <c r="X236" s="28"/>
       <c r="Y236" s="28"/>
       <c r="AQ236" s="28"/>
-      <c r="AY236" s="28"/>
+      <c r="AR236" s="28"/>
       <c r="BF236" s="29"/>
     </row>
     <row r="237" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2037,14 +2053,15 @@
       <c r="X237" s="28"/>
       <c r="Y237" s="28"/>
       <c r="AQ237" s="28"/>
-      <c r="AY237" s="28"/>
+      <c r="AR237" s="28"/>
+      <c r="AY237" s="35"/>
       <c r="BF237" s="29"/>
     </row>
     <row r="238" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B238" s="2"/>
       <c r="C238" s="30"/>
       <c r="D238" s="25"/>
-      <c r="E238" s="38"/>
+      <c r="E238" s="37"/>
       <c r="F238" s="43"/>
       <c r="G238" s="43"/>
       <c r="H238" s="49"/>
@@ -2064,8 +2081,8 @@
     <row r="239" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B239" s="2"/>
       <c r="C239" s="30"/>
-      <c r="D239" s="31"/>
-      <c r="E239" s="38"/>
+      <c r="D239" s="25"/>
+      <c r="E239" s="37"/>
       <c r="F239" s="43"/>
       <c r="G239" s="43"/>
       <c r="H239" s="49"/>
@@ -2085,8 +2102,8 @@
     <row r="240" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B240" s="2"/>
       <c r="C240" s="30"/>
-      <c r="D240" s="19"/>
-      <c r="E240" s="36"/>
+      <c r="D240" s="25"/>
+      <c r="E240" s="38"/>
       <c r="F240" s="43"/>
       <c r="G240" s="43"/>
       <c r="H240" s="49"/>
@@ -2099,13 +2116,15 @@
       <c r="W240" s="28"/>
       <c r="X240" s="28"/>
       <c r="Y240" s="28"/>
+      <c r="AQ240" s="28"/>
+      <c r="AY240" s="28"/>
       <c r="BF240" s="29"/>
     </row>
     <row r="241" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B241" s="2"/>
-      <c r="C241" s="17"/>
-      <c r="D241" s="19"/>
-      <c r="E241" s="36"/>
+      <c r="C241" s="30"/>
+      <c r="D241" s="31"/>
+      <c r="E241" s="38"/>
       <c r="F241" s="43"/>
       <c r="G241" s="43"/>
       <c r="H241" s="49"/>
@@ -2118,12 +2137,14 @@
       <c r="W241" s="28"/>
       <c r="X241" s="28"/>
       <c r="Y241" s="28"/>
+      <c r="AQ241" s="28"/>
+      <c r="AY241" s="28"/>
       <c r="BF241" s="29"/>
     </row>
     <row r="242" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B242" s="2"/>
       <c r="C242" s="30"/>
-      <c r="D242" s="31"/>
+      <c r="D242" s="19"/>
       <c r="E242" s="36"/>
       <c r="F242" s="43"/>
       <c r="G242" s="43"/>
@@ -2141,9 +2162,9 @@
     </row>
     <row r="243" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B243" s="2"/>
-      <c r="C243" s="30"/>
-      <c r="D243" s="25"/>
-      <c r="E243" s="37"/>
+      <c r="C243" s="17"/>
+      <c r="D243" s="19"/>
+      <c r="E243" s="36"/>
       <c r="F243" s="43"/>
       <c r="G243" s="43"/>
       <c r="H243" s="49"/>
@@ -2161,8 +2182,8 @@
     <row r="244" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B244" s="2"/>
       <c r="C244" s="30"/>
-      <c r="D244" s="25"/>
-      <c r="E244" s="37"/>
+      <c r="D244" s="31"/>
+      <c r="E244" s="36"/>
       <c r="F244" s="43"/>
       <c r="G244" s="43"/>
       <c r="H244" s="49"/>
@@ -2172,7 +2193,7 @@
       <c r="T244" s="28"/>
       <c r="U244" s="28"/>
       <c r="V244" s="28"/>
-      <c r="W244" s="5"/>
+      <c r="W244" s="28"/>
       <c r="X244" s="28"/>
       <c r="Y244" s="28"/>
       <c r="BF244" s="29"/>
@@ -2191,7 +2212,7 @@
       <c r="T245" s="28"/>
       <c r="U245" s="28"/>
       <c r="V245" s="28"/>
-      <c r="W245" s="5"/>
+      <c r="W245" s="28"/>
       <c r="X245" s="28"/>
       <c r="Y245" s="28"/>
       <c r="BF245" s="29"/>
@@ -2200,7 +2221,7 @@
       <c r="B246" s="2"/>
       <c r="C246" s="30"/>
       <c r="D246" s="25"/>
-      <c r="E246" s="36"/>
+      <c r="E246" s="37"/>
       <c r="F246" s="43"/>
       <c r="G246" s="43"/>
       <c r="H246" s="49"/>
@@ -2218,8 +2239,8 @@
     <row r="247" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B247" s="2"/>
       <c r="C247" s="30"/>
-      <c r="D247" s="19"/>
-      <c r="E247" s="36"/>
+      <c r="D247" s="25"/>
+      <c r="E247" s="37"/>
       <c r="F247" s="43"/>
       <c r="G247" s="43"/>
       <c r="H247" s="49"/>
@@ -2237,7 +2258,7 @@
     <row r="248" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B248" s="2"/>
       <c r="C248" s="30"/>
-      <c r="D248" s="19"/>
+      <c r="D248" s="25"/>
       <c r="E248" s="36"/>
       <c r="F248" s="43"/>
       <c r="G248" s="43"/>
@@ -2253,11 +2274,43 @@
       <c r="Y248" s="28"/>
       <c r="BF248" s="29"/>
     </row>
-    <row r="249" spans="2:58" x14ac:dyDescent="0.25">
-      <c r="C249" s="17"/>
-    </row>
-    <row r="250" spans="2:58" x14ac:dyDescent="0.25">
-      <c r="C250" s="17"/>
+    <row r="249" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B249" s="2"/>
+      <c r="C249" s="30"/>
+      <c r="D249" s="19"/>
+      <c r="E249" s="36"/>
+      <c r="F249" s="43"/>
+      <c r="G249" s="43"/>
+      <c r="H249" s="49"/>
+      <c r="I249" s="52"/>
+      <c r="O249" s="27"/>
+      <c r="S249" s="28"/>
+      <c r="T249" s="28"/>
+      <c r="U249" s="28"/>
+      <c r="V249" s="28"/>
+      <c r="W249" s="5"/>
+      <c r="X249" s="28"/>
+      <c r="Y249" s="28"/>
+      <c r="BF249" s="29"/>
+    </row>
+    <row r="250" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B250" s="2"/>
+      <c r="C250" s="30"/>
+      <c r="D250" s="19"/>
+      <c r="E250" s="36"/>
+      <c r="F250" s="43"/>
+      <c r="G250" s="43"/>
+      <c r="H250" s="49"/>
+      <c r="I250" s="52"/>
+      <c r="O250" s="27"/>
+      <c r="S250" s="28"/>
+      <c r="T250" s="28"/>
+      <c r="U250" s="28"/>
+      <c r="V250" s="28"/>
+      <c r="W250" s="5"/>
+      <c r="X250" s="28"/>
+      <c r="Y250" s="28"/>
+      <c r="BF250" s="29"/>
     </row>
     <row r="251" spans="2:58" x14ac:dyDescent="0.25">
       <c r="C251" s="17"/>
@@ -2265,49 +2318,17 @@
     <row r="252" spans="2:58" x14ac:dyDescent="0.25">
       <c r="C252" s="17"/>
     </row>
-    <row r="253" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B253" s="2"/>
+    <row r="253" spans="2:58" x14ac:dyDescent="0.25">
       <c r="C253" s="17"/>
-      <c r="D253" s="33"/>
-      <c r="E253" s="26"/>
-      <c r="F253" s="43"/>
-      <c r="G253" s="43"/>
-      <c r="H253" s="49"/>
-      <c r="I253" s="52"/>
-      <c r="O253" s="27"/>
-      <c r="S253" s="28"/>
-      <c r="T253" s="28"/>
-      <c r="U253" s="28"/>
-      <c r="V253" s="28"/>
-      <c r="W253" s="28"/>
-      <c r="X253" s="28"/>
-      <c r="Y253" s="28"/>
-      <c r="BF253" s="29"/>
-    </row>
-    <row r="254" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B254" s="2"/>
-      <c r="C254" s="30"/>
-      <c r="D254" s="31"/>
-      <c r="E254" s="36"/>
-      <c r="F254" s="43"/>
-      <c r="G254" s="43"/>
-      <c r="H254" s="49"/>
-      <c r="I254" s="52"/>
-      <c r="O254" s="27"/>
-      <c r="S254" s="28"/>
-      <c r="T254" s="28"/>
-      <c r="U254" s="28"/>
-      <c r="V254" s="28"/>
-      <c r="W254" s="28"/>
-      <c r="X254" s="28"/>
-      <c r="Y254" s="28"/>
-      <c r="BF254" s="29"/>
+    </row>
+    <row r="254" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="C254" s="17"/>
     </row>
     <row r="255" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B255" s="2"/>
-      <c r="C255" s="30"/>
-      <c r="D255" s="25"/>
-      <c r="E255" s="34"/>
+      <c r="C255" s="17"/>
+      <c r="D255" s="33"/>
+      <c r="E255" s="26"/>
       <c r="F255" s="43"/>
       <c r="G255" s="43"/>
       <c r="H255" s="49"/>
@@ -2325,8 +2346,8 @@
     <row r="256" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B256" s="2"/>
       <c r="C256" s="30"/>
-      <c r="D256" s="25"/>
-      <c r="E256" s="26"/>
+      <c r="D256" s="31"/>
+      <c r="E256" s="36"/>
       <c r="F256" s="43"/>
       <c r="G256" s="43"/>
       <c r="H256" s="49"/>
@@ -2358,14 +2379,13 @@
       <c r="W257" s="28"/>
       <c r="X257" s="28"/>
       <c r="Y257" s="28"/>
-      <c r="AQ257" s="28"/>
       <c r="BF257" s="29"/>
     </row>
     <row r="258" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B258" s="2"/>
       <c r="C258" s="30"/>
       <c r="D258" s="25"/>
-      <c r="E258" s="34"/>
+      <c r="E258" s="26"/>
       <c r="F258" s="43"/>
       <c r="G258" s="43"/>
       <c r="H258" s="49"/>
@@ -2378,7 +2398,6 @@
       <c r="W258" s="28"/>
       <c r="X258" s="28"/>
       <c r="Y258" s="28"/>
-      <c r="AQ258" s="28"/>
       <c r="BF258" s="29"/>
     </row>
     <row r="259" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2419,7 +2438,6 @@
       <c r="X260" s="28"/>
       <c r="Y260" s="28"/>
       <c r="AQ260" s="28"/>
-      <c r="AR260" s="28"/>
       <c r="BF260" s="29"/>
     </row>
     <row r="261" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2440,8 +2458,6 @@
       <c r="X261" s="28"/>
       <c r="Y261" s="28"/>
       <c r="AQ261" s="28"/>
-      <c r="AR261" s="28"/>
-      <c r="AY261" s="35"/>
       <c r="BF261" s="29"/>
     </row>
     <row r="262" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2462,7 +2478,7 @@
       <c r="X262" s="28"/>
       <c r="Y262" s="28"/>
       <c r="AQ262" s="28"/>
-      <c r="AY262" s="28"/>
+      <c r="AR262" s="28"/>
       <c r="BF262" s="29"/>
     </row>
     <row r="263" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2483,7 +2499,8 @@
       <c r="X263" s="28"/>
       <c r="Y263" s="28"/>
       <c r="AQ263" s="28"/>
-      <c r="AY263" s="28"/>
+      <c r="AR263" s="28"/>
+      <c r="AY263" s="35"/>
       <c r="BF263" s="29"/>
     </row>
     <row r="264" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
@@ -2553,7 +2570,7 @@
       <c r="B267" s="2"/>
       <c r="C267" s="30"/>
       <c r="D267" s="25"/>
-      <c r="E267" s="32"/>
+      <c r="E267" s="34"/>
       <c r="F267" s="43"/>
       <c r="G267" s="43"/>
       <c r="H267" s="49"/>
@@ -2573,8 +2590,8 @@
     <row r="268" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B268" s="2"/>
       <c r="C268" s="30"/>
-      <c r="D268" s="19"/>
-      <c r="E268" s="36"/>
+      <c r="D268" s="25"/>
+      <c r="E268" s="34"/>
       <c r="F268" s="43"/>
       <c r="G268" s="43"/>
       <c r="H268" s="49"/>
@@ -2587,53 +2604,57 @@
       <c r="W268" s="28"/>
       <c r="X268" s="28"/>
       <c r="Y268" s="28"/>
+      <c r="AQ268" s="28"/>
+      <c r="AY268" s="28"/>
       <c r="BF268" s="29"/>
     </row>
-    <row r="269" spans="2:58" x14ac:dyDescent="0.25">
+    <row r="269" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B269" s="2"/>
       <c r="C269" s="30"/>
-      <c r="D269" s="3"/>
-    </row>
-    <row r="270" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D269" s="25"/>
+      <c r="E269" s="32"/>
+      <c r="F269" s="43"/>
+      <c r="G269" s="43"/>
+      <c r="H269" s="49"/>
+      <c r="I269" s="52"/>
+      <c r="O269" s="27"/>
+      <c r="S269" s="28"/>
+      <c r="T269" s="28"/>
+      <c r="U269" s="28"/>
+      <c r="V269" s="28"/>
+      <c r="W269" s="28"/>
+      <c r="X269" s="28"/>
+      <c r="Y269" s="28"/>
+      <c r="AQ269" s="28"/>
+      <c r="AY269" s="28"/>
+      <c r="BF269" s="29"/>
+    </row>
+    <row r="270" spans="2:58" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B270" s="2"/>
-      <c r="C270" s="39"/>
-      <c r="D270" s="18"/>
-      <c r="E270" s="21"/>
-      <c r="F270" s="44"/>
-      <c r="G270" s="46"/>
-      <c r="H270" s="50"/>
-      <c r="I270" s="53"/>
-      <c r="O270" s="15"/>
-      <c r="S270" s="5"/>
-      <c r="T270" s="5"/>
-      <c r="U270" s="5"/>
-      <c r="V270" s="5"/>
-      <c r="W270" s="5"/>
-      <c r="X270" s="5"/>
-      <c r="Y270" s="5"/>
-      <c r="BF270" s="16"/>
-    </row>
-    <row r="271" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B271" s="7"/>
-      <c r="C271" s="10"/>
-      <c r="D271" s="18"/>
-      <c r="E271" s="21"/>
-      <c r="F271" s="44"/>
-      <c r="G271" s="46"/>
-      <c r="H271" s="50"/>
-      <c r="I271" s="53"/>
-      <c r="O271" s="15"/>
-      <c r="S271" s="5"/>
-      <c r="T271" s="5"/>
-      <c r="U271" s="5"/>
-      <c r="V271" s="5"/>
-      <c r="W271" s="5"/>
-      <c r="X271" s="5"/>
-      <c r="Y271" s="5"/>
-      <c r="BF271" s="16"/>
+      <c r="C270" s="30"/>
+      <c r="D270" s="19"/>
+      <c r="E270" s="36"/>
+      <c r="F270" s="43"/>
+      <c r="G270" s="43"/>
+      <c r="H270" s="49"/>
+      <c r="I270" s="52"/>
+      <c r="O270" s="27"/>
+      <c r="S270" s="28"/>
+      <c r="T270" s="28"/>
+      <c r="U270" s="28"/>
+      <c r="V270" s="28"/>
+      <c r="W270" s="28"/>
+      <c r="X270" s="28"/>
+      <c r="Y270" s="28"/>
+      <c r="BF270" s="29"/>
+    </row>
+    <row r="271" spans="2:58" x14ac:dyDescent="0.25">
+      <c r="C271" s="30"/>
+      <c r="D271" s="3"/>
     </row>
     <row r="272" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B272" s="2"/>
-      <c r="C272" s="17"/>
+      <c r="C272" s="39"/>
       <c r="D272" s="18"/>
       <c r="E272" s="21"/>
       <c r="F272" s="44"/>
@@ -2651,8 +2672,8 @@
       <c r="BF272" s="16"/>
     </row>
     <row r="273" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B273" s="2"/>
-      <c r="C273" s="17"/>
+      <c r="B273" s="7"/>
+      <c r="C273" s="10"/>
       <c r="D273" s="18"/>
       <c r="E273" s="21"/>
       <c r="F273" s="44"/>
@@ -2690,7 +2711,7 @@
     </row>
     <row r="275" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B275" s="2"/>
-      <c r="C275" s="39"/>
+      <c r="C275" s="17"/>
       <c r="D275" s="18"/>
       <c r="E275" s="21"/>
       <c r="F275" s="44"/>
@@ -2709,7 +2730,7 @@
     </row>
     <row r="276" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B276" s="2"/>
-      <c r="C276" s="10"/>
+      <c r="C276" s="17"/>
       <c r="D276" s="18"/>
       <c r="E276" s="21"/>
       <c r="F276" s="44"/>
@@ -2728,7 +2749,7 @@
     </row>
     <row r="277" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B277" s="2"/>
-      <c r="C277" s="10"/>
+      <c r="C277" s="39"/>
       <c r="D277" s="18"/>
       <c r="E277" s="21"/>
       <c r="F277" s="44"/>
@@ -2782,6 +2803,44 @@
       <c r="X279" s="5"/>
       <c r="Y279" s="5"/>
       <c r="BF279" s="16"/>
+    </row>
+    <row r="280" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B280" s="2"/>
+      <c r="C280" s="10"/>
+      <c r="D280" s="18"/>
+      <c r="E280" s="21"/>
+      <c r="F280" s="44"/>
+      <c r="G280" s="46"/>
+      <c r="H280" s="50"/>
+      <c r="I280" s="53"/>
+      <c r="O280" s="15"/>
+      <c r="S280" s="5"/>
+      <c r="T280" s="5"/>
+      <c r="U280" s="5"/>
+      <c r="V280" s="5"/>
+      <c r="W280" s="5"/>
+      <c r="X280" s="5"/>
+      <c r="Y280" s="5"/>
+      <c r="BF280" s="16"/>
+    </row>
+    <row r="281" spans="2:58" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B281" s="2"/>
+      <c r="C281" s="10"/>
+      <c r="D281" s="18"/>
+      <c r="E281" s="21"/>
+      <c r="F281" s="44"/>
+      <c r="G281" s="46"/>
+      <c r="H281" s="50"/>
+      <c r="I281" s="53"/>
+      <c r="O281" s="15"/>
+      <c r="S281" s="5"/>
+      <c r="T281" s="5"/>
+      <c r="U281" s="5"/>
+      <c r="V281" s="5"/>
+      <c r="W281" s="5"/>
+      <c r="X281" s="5"/>
+      <c r="Y281" s="5"/>
+      <c r="BF281" s="16"/>
     </row>
   </sheetData>
   <sortState ref="D257:U260">

</xml_diff>